<commit_message>
Added Validation Logic in Dispatcher.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b498711e3aabb8c/Documents/UiPath/Insurance_Claim_Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{2F4F66D7-7208-4AEF-90E5-B69C4AEAB423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC0A9EC5-0A67-4FC7-877D-C2811BB2BD88}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{2F4F66D7-7208-4AEF-90E5-B69C4AEAB423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB8CD4A2-4B0B-45E4-8921-A5ECC9E75375}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -165,6 +165,15 @@
   </si>
   <si>
     <t>Insurance_Dispatcher_BusinessExceptionFIlePath</t>
+  </si>
+  <si>
+    <t>Insurance_Dispatcher_BlackListedExcelPath</t>
+  </si>
+  <si>
+    <t>Insurance_Dispatcher_TreatmenttypelistPath</t>
+  </si>
+  <si>
+    <t>Insurance_Dispatcher_RejectedOrManualClaimsExcelPath</t>
   </si>
 </sst>
 </file>
@@ -546,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2791,13 +2800,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.33203125" customWidth="1"/>
     <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
@@ -2854,9 +2863,30 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Insurance Dispatcher Retry Mechanism Added.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{2F4F66D7-7208-4AEF-90E5-B69C4AEAB423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB8CD4A2-4B0B-45E4-8921-A5ECC9E75375}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2800,7 +2800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>